<commit_message>
ADD menu string edit ADD result to xlsx file
</commit_message>
<xml_diff>
--- a/df.xlsx
+++ b/df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>날짜</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>구분</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>메뉴</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>칼로리</t>
         </is>
       </c>
     </row>
@@ -456,17 +466,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>서울고</t>
+          <t>휘봉고등학교</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>20210104</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>중식</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>밥,국</t>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>현미밥, 청양콩나물국, 청포묵무침, 제육볶음, 배추김치, 귤</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>356.7 Kcal</t>
         </is>
       </c>
     </row>
@@ -476,17 +496,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>평택고</t>
+          <t>휘경여자고등학교</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>석식</t>
+          <t>20210104</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>밥,국,찌개</t>
+          <t>중식</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>옥수수밥, 쇠고기샤브샤브국, 진미채고추장볶음, 치즈불닭, 굴림만두, 깍두기, 자몽데르뜨</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>801.3 Kcal</t>
         </is>
       </c>
     </row>
@@ -496,17 +526,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>서울고</t>
+          <t>휘경여자고등학교</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>20210105</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>중식</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>밥,국</t>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>흑미밥, 사골조랭이고기만두국, 도토리묵야채무침, 스팸감자구이, 어향동태강정, 배추김치</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>935.2 Kcal</t>
         </is>
       </c>
     </row>
@@ -516,17 +556,57 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>평택고</t>
+          <t>휘경공업고등학교</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>석식</t>
+          <t>20210104</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>밥,국,찌개</t>
+          <t>중식</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>칼슘강화강낭콩밥, 맑은콩나물국, 시금치나물무침, 닭볶음탕, 어묵피망볶음, 깍두기</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>1022.3 Kcal</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>휘경공업고등학교</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>20210105</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>중식</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>칼슘강화현미밥, 아욱국, 돈등뼈김치찜, 갈릭난*커리소스, 깍두기, 리코타치즈샐러드</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>1099.0 Kcal</t>
         </is>
       </c>
     </row>

</xml_diff>